<commit_message>
update experimental results without normalization for old dataset (Wong3)
</commit_message>
<xml_diff>
--- a/experiment_results/20201206_AGGREGATION_AVERAGE_ADDITION_NORMALIZATION3/BankAccountTP/4wise/0.95_.xlsx
+++ b/experiment_results/20201206_AGGREGATION_AVERAGE_ADDITION_NORMALIZATION3/BankAccountTP/4wise/0.95_.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="op2" sheetId="1" r:id="rId1"/>
+    <sheet name="wong3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -502,10 +502,10 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>76</v>
@@ -531,19 +531,19 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>23</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>76</v>
@@ -578,10 +578,10 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G4">
         <v>76</v>
@@ -607,7 +607,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -616,10 +616,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>76</v>
@@ -654,10 +654,10 @@
         <v>11</v>
       </c>
       <c r="E6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6">
         <v>76</v>
@@ -692,10 +692,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G7">
         <v>76</v>
@@ -721,19 +721,19 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G8">
         <v>76</v>
@@ -768,10 +768,10 @@
         <v>14</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F9">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -806,10 +806,10 @@
         <v>16</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G10">
         <v>76</v>
@@ -911,19 +911,19 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>23</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G13">
         <v>76</v>
@@ -949,19 +949,19 @@
         <v>24</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>24</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G14">
         <v>76</v>
@@ -996,10 +996,10 @@
         <v>34</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G15">
         <v>76</v>
@@ -1034,10 +1034,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G16">
         <v>76</v>
@@ -1101,19 +1101,19 @@
         <v>28</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>11</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G18">
         <v>76</v>
@@ -1215,19 +1215,19 @@
         <v>31</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21">
         <v>21</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G21">
         <v>76</v>
@@ -1253,19 +1253,19 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="G22">
         <v>76</v>

</xml_diff>